<commit_message>
Asset Patch - work fillingout edc-patcher.
</commit_message>
<xml_diff>
--- a/fsharp/asset-patch/edc-patcher/excel-sample/WorkListSample.xlsx
+++ b/fsharp/asset-patch/edc-patcher/excel-sample/WorkListSample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\work\asset-trafo\fsharp\asset-patch\edc-patcher\excel-sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\github\asset-trafo\fsharp\asset-patch\edc-patcher\excel-sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71940EFF-2A57-4F02-9271-2B9277B365A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{807693B4-978B-4811-9074-EC74250753F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F9EA631D-0435-45C1-B7CC-C2C1FD7F9DA1}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>BRI01</t>
   </si>
@@ -66,7 +66,88 @@
     <t>PDB2981/XK</t>
   </si>
   <si>
-    <t>Root S4 FuncLoc</t>
+    <t>AI2 Site Reference</t>
+  </si>
+  <si>
+    <t>S4 Root FuncLoc</t>
+  </si>
+  <si>
+    <t>SAI00023001</t>
+  </si>
+  <si>
+    <t>AI2 Equipment SAI Number</t>
+  </si>
+  <si>
+    <t>AI2 Equipment PLI Code</t>
+  </si>
+  <si>
+    <t>SAI00023450</t>
+  </si>
+  <si>
+    <t>PLI00004561</t>
+  </si>
+  <si>
+    <t>Memo Line</t>
+  </si>
+  <si>
+    <t>Relay 1 Function</t>
+  </si>
+  <si>
+    <t>Relay 1 On</t>
+  </si>
+  <si>
+    <t>Relay 1 Off</t>
+  </si>
+  <si>
+    <t>Relay 2 Function</t>
+  </si>
+  <si>
+    <t>Relay 2 On</t>
+  </si>
+  <si>
+    <t>Relay 2 Off</t>
+  </si>
+  <si>
+    <t>Relay 3 Function</t>
+  </si>
+  <si>
+    <t>Relay 3 On</t>
+  </si>
+  <si>
+    <t>Relay 3 Off</t>
+  </si>
+  <si>
+    <t>Relay 4 Function</t>
+  </si>
+  <si>
+    <t>Relay 4 On</t>
+  </si>
+  <si>
+    <t>Relay 4 Off</t>
+  </si>
+  <si>
+    <t>Relay 5 Function</t>
+  </si>
+  <si>
+    <t>Relay 5 On</t>
+  </si>
+  <si>
+    <t>Relay 5 Off</t>
+  </si>
+  <si>
+    <t>Relay 6 Function</t>
+  </si>
+  <si>
+    <t>Relay 6 On</t>
+  </si>
+  <si>
+    <t>Relay 6 Off</t>
+  </si>
+  <si>
+    <t>LOSS OF ECHO</t>
+  </si>
+  <si>
+    <t>Install Date</t>
   </si>
 </sst>
 </file>
@@ -102,8 +183,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,58 +500,149 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1DA0B99-BC0C-4E9D-804B-8BEC68776EFA}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" customWidth="1"/>
+    <col min="7" max="7" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" t="s">
+        <v>30</v>
+      </c>
+      <c r="X1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="1">
+        <v>43679</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>10</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Asset Patch: EdcPatcher more work filling out the template.
</commit_message>
<xml_diff>
--- a/fsharp/asset-patch/edc-patcher/excel-sample/WorkListSample.xlsx
+++ b/fsharp/asset-patch/edc-patcher/excel-sample/WorkListSample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\github\asset-trafo\fsharp\asset-patch\edc-patcher\excel-sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\work\asset-trafo\fsharp\asset-patch\edc-patcher\excel-sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{807693B4-978B-4811-9074-EC74250753F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD72C32A-59BD-4306-83A2-EC2AB975F5F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F9EA631D-0435-45C1-B7CC-C2C1FD7F9DA1}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>BRI01</t>
   </si>
@@ -148,6 +148,18 @@
   </si>
   <si>
     <t>Install Date</t>
+  </si>
+  <si>
+    <t>Transducer Model</t>
+  </si>
+  <si>
+    <t>XRS-5</t>
+  </si>
+  <si>
+    <t>Transducer Serial Number</t>
+  </si>
+  <si>
+    <t>2007/234500</t>
   </si>
 </sst>
 </file>
@@ -500,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1DA0B99-BC0C-4E9D-804B-8BEC68776EFA}">
-  <dimension ref="A1:AC2"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,11 +529,12 @@
     <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="13.85546875" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -553,64 +566,70 @@
         <v>7</v>
       </c>
       <c r="K1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>19</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>20</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>21</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>22</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>24</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>25</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>26</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>27</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>28</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>29</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>30</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>32</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>33</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>34</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>35</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -641,7 +660,13 @@
       <c r="J2" t="s">
         <v>10</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="K2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC2" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
asset-patch - minor changes as I look to making the edc-patcher 'robust'.
</commit_message>
<xml_diff>
--- a/fsharp/asset-patch/edc-patcher/excel-sample/WorkListSample.xlsx
+++ b/fsharp/asset-patch/edc-patcher/excel-sample/WorkListSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\work\asset-trafo\fsharp\asset-patch\edc-patcher\excel-sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD72C32A-59BD-4306-83A2-EC2AB975F5F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E82BC28-BDA5-4E57-9246-879B25B64E48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F9EA631D-0435-45C1-B7CC-C2C1FD7F9DA1}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>BRI01</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>2007/234500</t>
+  </si>
+  <si>
+    <t>S4 System Name</t>
+  </si>
+  <si>
+    <t>EA Event Duration Monitoring</t>
   </si>
 </sst>
 </file>
@@ -512,29 +518,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1DA0B99-BC0C-4E9D-804B-8BEC68776EFA}">
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" customWidth="1"/>
-    <col min="7" max="7" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="13.85546875" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" customWidth="1"/>
+    <col min="8" max="8" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.85546875" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -542,94 +549,97 @@
         <v>11</v>
       </c>
       <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>38</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>39</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>41</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>18</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>19</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>20</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>22</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>23</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>24</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>25</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>26</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>27</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>28</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>29</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>30</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>31</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>32</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>33</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>34</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>35</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -637,36 +647,39 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>43679</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>10</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>40</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>42</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
asset-patch - EdcPatcher - changed the format of the Excel input sample for the type provider.
</commit_message>
<xml_diff>
--- a/fsharp/asset-patch/edc-patcher/excel-sample/WorkListSample.xlsx
+++ b/fsharp/asset-patch/edc-patcher/excel-sample/WorkListSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\work\asset-trafo\fsharp\asset-patch\edc-patcher\excel-sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E82BC28-BDA5-4E57-9246-879B25B64E48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD64689-16E3-4942-AD59-CF9D7370CE03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F9EA631D-0435-45C1-B7CC-C2C1FD7F9DA1}"/>
   </bookViews>
@@ -31,62 +31,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
-  <si>
-    <t>BRI01</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="90">
   <si>
     <t>NGR</t>
   </si>
   <si>
-    <t>ND1128168190</t>
-  </si>
-  <si>
     <t>Level Controller Name</t>
   </si>
   <si>
-    <t>Storm Overflow Level Monitor Loop</t>
-  </si>
-  <si>
-    <t>Manufacturer</t>
-  </si>
-  <si>
-    <t>Model</t>
-  </si>
-  <si>
-    <t>Serial Number</t>
-  </si>
-  <si>
     <t>SIEMENS</t>
   </si>
   <si>
-    <t>HYDRORANGER 200</t>
-  </si>
-  <si>
-    <t>PDB2981/XK</t>
-  </si>
-  <si>
-    <t>AI2 Site Reference</t>
-  </si>
-  <si>
     <t>S4 Root FuncLoc</t>
   </si>
   <si>
-    <t>SAI00023001</t>
-  </si>
-  <si>
     <t>AI2 Equipment SAI Number</t>
   </si>
   <si>
     <t>AI2 Equipment PLI Code</t>
   </si>
   <si>
-    <t>SAI00023450</t>
-  </si>
-  <si>
-    <t>PLI00004561</t>
-  </si>
-  <si>
     <t>Memo Line</t>
   </si>
   <si>
@@ -159,20 +123,191 @@
     <t>Transducer Serial Number</t>
   </si>
   <si>
-    <t>2007/234500</t>
-  </si>
-  <si>
     <t>S4 System Name</t>
   </si>
   <si>
-    <t>EA Event Duration Monitoring</t>
+    <t>AI2 Common Name</t>
+  </si>
+  <si>
+    <t>Controller Serial Number</t>
+  </si>
+  <si>
+    <t>Controller Model</t>
+  </si>
+  <si>
+    <t>Controller Manufacturer</t>
+  </si>
+  <si>
+    <t>UNDESIGNATED LEVEL ALARM</t>
+  </si>
+  <si>
+    <t>XPS-15</t>
+  </si>
+  <si>
+    <t>AI2 Root Reference</t>
+  </si>
+  <si>
+    <t>S4 Equipment FuncLoc</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>SAI00000001</t>
+  </si>
+  <si>
+    <t>SAI00000002</t>
+  </si>
+  <si>
+    <t>SAI00000003</t>
+  </si>
+  <si>
+    <t>SAI00000004</t>
+  </si>
+  <si>
+    <t>SAI00000005</t>
+  </si>
+  <si>
+    <t>SAI00000006</t>
+  </si>
+  <si>
+    <t>SAI00000007</t>
+  </si>
+  <si>
+    <t>SAI00000008</t>
+  </si>
+  <si>
+    <t>SAI00000009</t>
+  </si>
+  <si>
+    <t>PLI00000001</t>
+  </si>
+  <si>
+    <t>PLI00000002</t>
+  </si>
+  <si>
+    <t>PLI00000003</t>
+  </si>
+  <si>
+    <t>PLI00000004</t>
+  </si>
+  <si>
+    <t>PLI00000005</t>
+  </si>
+  <si>
+    <t>PLI00000006</t>
+  </si>
+  <si>
+    <t>PLI00000007</t>
+  </si>
+  <si>
+    <t>PLI00000008</t>
+  </si>
+  <si>
+    <t>PLI00000009</t>
+  </si>
+  <si>
+    <t>PLI00000010</t>
+  </si>
+  <si>
+    <t>SAI00000010</t>
+  </si>
+  <si>
+    <t>SE6161273406</t>
+  </si>
+  <si>
+    <t>SE4856638339</t>
+  </si>
+  <si>
+    <t>Zzzzzzz should add equipment to an existing FuncLoc (no new funclocs)</t>
+  </si>
+  <si>
+    <t>Installed on scheme Z003 Plant Refurbishment 2019</t>
+  </si>
+  <si>
+    <t>ABC/12001</t>
+  </si>
+  <si>
+    <t>ABC/12003</t>
+  </si>
+  <si>
+    <t>ABC/12005</t>
+  </si>
+  <si>
+    <t>ABC/12007</t>
+  </si>
+  <si>
+    <t>ABC/12009</t>
+  </si>
+  <si>
+    <t>AB/10001</t>
+  </si>
+  <si>
+    <t>AB/10002</t>
+  </si>
+  <si>
+    <t>AB/10003</t>
+  </si>
+  <si>
+    <t>AB/10004</t>
+  </si>
+  <si>
+    <t>AB/10005</t>
+  </si>
+  <si>
+    <t>AB/10006</t>
+  </si>
+  <si>
+    <t>AB/10007</t>
+  </si>
+  <si>
+    <t>AB/10008</t>
+  </si>
+  <si>
+    <t>AB/10009</t>
+  </si>
+  <si>
+    <t>AB/10010</t>
+  </si>
+  <si>
+    <t>CONTROLLER PLUS</t>
+  </si>
+  <si>
+    <t>CONTROLLER 2000</t>
+  </si>
+  <si>
+    <t>Level Monitoring Loop</t>
+  </si>
+  <si>
+    <t>High Level Monitoring Loop</t>
+  </si>
+  <si>
+    <t>Overflow Monitoring Loop</t>
+  </si>
+  <si>
+    <t>On Site Monitoring System</t>
+  </si>
+  <si>
+    <t>XYZ01-EDC-LQD-RGM</t>
+  </si>
+  <si>
+    <t>XYZ01-EDC-LQD</t>
+  </si>
+  <si>
+    <t>XYZ01</t>
+  </si>
+  <si>
+    <t>XYZ01-EDC-LQD-RGM-SYS01</t>
+  </si>
+  <si>
+    <t>WESTLAKE/INCOMING LANE/EQUIPMENT: LEVEL MONITORING UNIT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,13 +315,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -201,9 +354,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,172 +674,892 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1DA0B99-BC0C-4E9D-804B-8BEC68776EFA}">
-  <dimension ref="A1:AF2"/>
+  <sheetPr transitionEvaluation="1"/>
+  <dimension ref="A1:AI11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="145" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" customWidth="1"/>
-    <col min="8" max="8" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="13.85546875" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" customWidth="1"/>
+    <col min="15" max="15" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="61.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="68.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>8</v>
+      </c>
+      <c r="R1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S1" t="s">
+        <v>10</v>
+      </c>
+      <c r="T1" t="s">
+        <v>11</v>
+      </c>
+      <c r="U1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="V1" t="s">
+        <v>13</v>
+      </c>
+      <c r="W1" t="s">
+        <v>14</v>
+      </c>
+      <c r="X1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J2" s="1">
+        <v>43726</v>
+      </c>
+      <c r="K2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M2" t="s">
+        <v>69</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2">
+        <v>1.5</v>
+      </c>
+      <c r="R2">
+        <v>1.2</v>
+      </c>
+      <c r="S2" t="s">
+        <v>35</v>
+      </c>
+      <c r="T2">
+        <v>1.5</v>
+      </c>
+      <c r="U2">
+        <v>1.2</v>
+      </c>
+      <c r="V2" t="s">
+        <v>35</v>
+      </c>
+      <c r="W2">
+        <v>1.5</v>
+      </c>
+      <c r="X2">
+        <v>1.2</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z2">
+        <v>1.5</v>
+      </c>
+      <c r="AA2">
+        <v>1.2</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC2">
+        <v>1.5</v>
+      </c>
+      <c r="AD2">
+        <v>1.2</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF2">
+        <v>1.5</v>
+      </c>
+      <c r="AG2">
+        <v>1.2</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J3" s="1">
+        <v>43733</v>
+      </c>
+      <c r="K3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" t="s">
+        <v>80</v>
+      </c>
+      <c r="M3" t="s">
+        <v>70</v>
+      </c>
+      <c r="N3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" t="s">
+        <v>25</v>
+      </c>
+      <c r="S3" t="s">
+        <v>25</v>
+      </c>
+      <c r="V3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" s="1">
+        <v>43741</v>
+      </c>
+      <c r="K4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" t="s">
+        <v>80</v>
+      </c>
+      <c r="M4" t="s">
+        <v>71</v>
+      </c>
+      <c r="N4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
         <v>43</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>21</v>
-      </c>
-      <c r="R1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S1" t="s">
-        <v>23</v>
-      </c>
-      <c r="T1" t="s">
-        <v>24</v>
-      </c>
-      <c r="U1" t="s">
-        <v>25</v>
-      </c>
-      <c r="V1" t="s">
-        <v>26</v>
-      </c>
-      <c r="W1" t="s">
-        <v>27</v>
-      </c>
-      <c r="X1" t="s">
+      <c r="C5" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H5" t="s">
+        <v>84</v>
+      </c>
+      <c r="I5" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5" s="1">
+        <v>43768</v>
+      </c>
+      <c r="K5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" t="s">
+        <v>80</v>
+      </c>
+      <c r="M5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N5" t="s">
         <v>28</v>
       </c>
-      <c r="Y1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF1" t="s">
+      <c r="P5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5">
+        <v>1.5</v>
+      </c>
+      <c r="R5">
+        <v>1.2</v>
+      </c>
+      <c r="S5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T5">
+        <v>1.5</v>
+      </c>
+      <c r="U5">
+        <v>1.2</v>
+      </c>
+      <c r="V5" t="s">
+        <v>35</v>
+      </c>
+      <c r="W5">
+        <v>1.5</v>
+      </c>
+      <c r="X5">
+        <v>1.2</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z5">
+        <v>1.5</v>
+      </c>
+      <c r="AA5">
+        <v>1.2</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC5">
+        <v>1.5</v>
+      </c>
+      <c r="AD5">
+        <v>1.2</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF5">
+        <v>1.5</v>
+      </c>
+      <c r="AG5">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" t="s">
+        <v>84</v>
+      </c>
+      <c r="I6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J6" s="1">
+        <v>43749</v>
+      </c>
+      <c r="K6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" t="s">
+        <v>79</v>
+      </c>
+      <c r="M6" t="s">
+        <v>73</v>
+      </c>
+      <c r="N6" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" t="s">
+        <v>66</v>
+      </c>
+      <c r="P6" t="s">
+        <v>25</v>
+      </c>
+      <c r="S6" t="s">
+        <v>25</v>
+      </c>
+      <c r="V6" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H7" t="s">
+        <v>84</v>
+      </c>
+      <c r="I7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J7" s="1">
+        <v>43682</v>
+      </c>
+      <c r="K7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" t="s">
+        <v>80</v>
+      </c>
+      <c r="M7" t="s">
+        <v>74</v>
+      </c>
+      <c r="N7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H8" t="s">
+        <v>84</v>
+      </c>
+      <c r="I8" t="s">
+        <v>83</v>
+      </c>
+      <c r="J8" s="1">
+        <v>43697</v>
+      </c>
+      <c r="K8" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1">
-        <v>43679</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" t="s">
-        <v>40</v>
-      </c>
-      <c r="M2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>37</v>
+      <c r="L8" t="s">
+        <v>80</v>
+      </c>
+      <c r="M8" t="s">
+        <v>75</v>
+      </c>
+      <c r="N8" t="s">
+        <v>36</v>
+      </c>
+      <c r="O8" t="s">
+        <v>67</v>
+      </c>
+      <c r="P8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8">
+        <v>1.5</v>
+      </c>
+      <c r="R8">
+        <v>1.2</v>
+      </c>
+      <c r="S8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T8">
+        <v>1.5</v>
+      </c>
+      <c r="U8">
+        <v>1.2</v>
+      </c>
+      <c r="V8" t="s">
+        <v>35</v>
+      </c>
+      <c r="W8">
+        <v>1.5</v>
+      </c>
+      <c r="X8">
+        <v>1.2</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z8">
+        <v>1.5</v>
+      </c>
+      <c r="AA8">
+        <v>1.2</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC8">
+        <v>1.5</v>
+      </c>
+      <c r="AD8">
+        <v>1.2</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF8">
+        <v>1.5</v>
+      </c>
+      <c r="AG8">
+        <v>1.2</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI8" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" t="s">
+        <v>84</v>
+      </c>
+      <c r="I9" t="s">
+        <v>82</v>
+      </c>
+      <c r="J9" s="1">
+        <v>43769</v>
+      </c>
+      <c r="K9" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" t="s">
+        <v>80</v>
+      </c>
+      <c r="M9" t="s">
+        <v>76</v>
+      </c>
+      <c r="N9" t="s">
+        <v>36</v>
+      </c>
+      <c r="P9" t="s">
+        <v>25</v>
+      </c>
+      <c r="S9" t="s">
+        <v>25</v>
+      </c>
+      <c r="V9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I10" t="s">
+        <v>81</v>
+      </c>
+      <c r="J10" s="1">
+        <v>43677</v>
+      </c>
+      <c r="K10" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" t="s">
+        <v>80</v>
+      </c>
+      <c r="M10" t="s">
+        <v>77</v>
+      </c>
+      <c r="N10" t="s">
+        <v>36</v>
+      </c>
+      <c r="O10" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H11" t="s">
+        <v>84</v>
+      </c>
+      <c r="I11" t="s">
+        <v>81</v>
+      </c>
+      <c r="J11" s="1">
+        <v>43677</v>
+      </c>
+      <c r="K11" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" t="s">
+        <v>80</v>
+      </c>
+      <c r="M11" t="s">
+        <v>78</v>
+      </c>
+      <c r="N11" t="s">
+        <v>36</v>
+      </c>
+      <c r="P11" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q11">
+        <v>1.5</v>
+      </c>
+      <c r="R11">
+        <v>1.2</v>
+      </c>
+      <c r="S11" t="s">
+        <v>35</v>
+      </c>
+      <c r="T11">
+        <v>1.5</v>
+      </c>
+      <c r="U11">
+        <v>1.2</v>
+      </c>
+      <c r="V11" t="s">
+        <v>35</v>
+      </c>
+      <c r="W11">
+        <v>1.5</v>
+      </c>
+      <c r="X11">
+        <v>1.2</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z11">
+        <v>1.5</v>
+      </c>
+      <c r="AA11">
+        <v>1.2</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC11">
+        <v>1.5</v>
+      </c>
+      <c r="AD11">
+        <v>1.2</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF11">
+        <v>1.5</v>
+      </c>
+      <c r="AG11">
+        <v>1.2</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AI49">
+    <sortCondition ref="C2:C49"/>
+  </sortState>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>